<commit_message>
Implementado hasta la generacion de la matriz de ejemplos. Muchas funciones nuevas
</commit_message>
<xml_diff>
--- a/DatosEsp1/SP1213.xlsx
+++ b/DatosEsp1/SP1213.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="150">
   <si>
     <t>Div</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>30/03/13</t>
+  </si>
+  <si>
+    <t>31/03/13</t>
   </si>
 </sst>
 </file>
@@ -1283,11 +1286,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR285"/>
+  <dimension ref="A1:BR291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -61666,6 +61667,1278 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
+    <row r="286" spans="1:70">
+      <c r="A286" t="s">
+        <v>70</v>
+      </c>
+      <c r="B286" t="s">
+        <v>149</v>
+      </c>
+      <c r="C286" t="s">
+        <v>87</v>
+      </c>
+      <c r="D286" t="s">
+        <v>89</v>
+      </c>
+      <c r="E286">
+        <v>1</v>
+      </c>
+      <c r="F286">
+        <v>1</v>
+      </c>
+      <c r="G286" t="s">
+        <v>75</v>
+      </c>
+      <c r="H286">
+        <v>1</v>
+      </c>
+      <c r="I286">
+        <v>1</v>
+      </c>
+      <c r="J286" t="s">
+        <v>75</v>
+      </c>
+      <c r="K286">
+        <v>9</v>
+      </c>
+      <c r="L286">
+        <v>15</v>
+      </c>
+      <c r="M286">
+        <v>4</v>
+      </c>
+      <c r="N286">
+        <v>3</v>
+      </c>
+      <c r="O286">
+        <v>21</v>
+      </c>
+      <c r="P286">
+        <v>8</v>
+      </c>
+      <c r="Q286">
+        <v>6</v>
+      </c>
+      <c r="R286">
+        <v>7</v>
+      </c>
+      <c r="S286">
+        <v>3</v>
+      </c>
+      <c r="T286">
+        <v>3</v>
+      </c>
+      <c r="U286">
+        <v>0</v>
+      </c>
+      <c r="V286">
+        <v>0</v>
+      </c>
+      <c r="W286">
+        <v>1.73</v>
+      </c>
+      <c r="X286">
+        <v>3.6</v>
+      </c>
+      <c r="Y286">
+        <v>4.75</v>
+      </c>
+      <c r="Z286">
+        <v>1.75</v>
+      </c>
+      <c r="AA286">
+        <v>3.5</v>
+      </c>
+      <c r="AB286">
+        <v>4.75</v>
+      </c>
+      <c r="AC286">
+        <v>1.75</v>
+      </c>
+      <c r="AD286">
+        <v>3.5</v>
+      </c>
+      <c r="AE286">
+        <v>4.75</v>
+      </c>
+      <c r="AF286">
+        <v>1.8</v>
+      </c>
+      <c r="AG286">
+        <v>3.5</v>
+      </c>
+      <c r="AH286">
+        <v>4.2</v>
+      </c>
+      <c r="AI286">
+        <v>1.75</v>
+      </c>
+      <c r="AJ286">
+        <v>3.75</v>
+      </c>
+      <c r="AK286">
+        <v>4.5</v>
+      </c>
+      <c r="AL286">
+        <v>1.78</v>
+      </c>
+      <c r="AM286">
+        <v>3.82</v>
+      </c>
+      <c r="AN286">
+        <v>5.04</v>
+      </c>
+      <c r="AO286">
+        <v>1.8</v>
+      </c>
+      <c r="AP286">
+        <v>3.5</v>
+      </c>
+      <c r="AQ286">
+        <v>4.5</v>
+      </c>
+      <c r="AR286">
+        <v>1.8</v>
+      </c>
+      <c r="AS286">
+        <v>3.5</v>
+      </c>
+      <c r="AT286">
+        <v>4.8</v>
+      </c>
+      <c r="AU286">
+        <v>1.8</v>
+      </c>
+      <c r="AV286">
+        <v>3.75</v>
+      </c>
+      <c r="AW286">
+        <v>4.75</v>
+      </c>
+      <c r="AX286">
+        <v>1.8</v>
+      </c>
+      <c r="AY286">
+        <v>3.5</v>
+      </c>
+      <c r="AZ286">
+        <v>4.5</v>
+      </c>
+      <c r="BA286">
+        <v>38</v>
+      </c>
+      <c r="BB286">
+        <v>1.8</v>
+      </c>
+      <c r="BC286">
+        <v>1.75</v>
+      </c>
+      <c r="BD286">
+        <v>3.85</v>
+      </c>
+      <c r="BE286">
+        <v>3.58</v>
+      </c>
+      <c r="BF286">
+        <v>5.22</v>
+      </c>
+      <c r="BG286">
+        <v>4.74</v>
+      </c>
+      <c r="BH286">
+        <v>38</v>
+      </c>
+      <c r="BI286">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BJ286">
+        <v>1.92</v>
+      </c>
+      <c r="BK286">
+        <v>1.98</v>
+      </c>
+      <c r="BL286">
+        <v>1.88</v>
+      </c>
+      <c r="BM286">
+        <v>21</v>
+      </c>
+      <c r="BN286">
+        <v>-0.75</v>
+      </c>
+      <c r="BO286">
+        <v>2.02</v>
+      </c>
+      <c r="BP286">
+        <v>1.98</v>
+      </c>
+      <c r="BQ286">
+        <v>1.95</v>
+      </c>
+      <c r="BR286">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="287" spans="1:70">
+      <c r="A287" t="s">
+        <v>70</v>
+      </c>
+      <c r="B287" t="s">
+        <v>149</v>
+      </c>
+      <c r="C287" t="s">
+        <v>77</v>
+      </c>
+      <c r="D287" t="s">
+        <v>85</v>
+      </c>
+      <c r="E287">
+        <v>2</v>
+      </c>
+      <c r="F287">
+        <v>2</v>
+      </c>
+      <c r="G287" t="s">
+        <v>75</v>
+      </c>
+      <c r="H287">
+        <v>2</v>
+      </c>
+      <c r="I287">
+        <v>1</v>
+      </c>
+      <c r="J287" t="s">
+        <v>78</v>
+      </c>
+      <c r="K287">
+        <v>7</v>
+      </c>
+      <c r="L287">
+        <v>15</v>
+      </c>
+      <c r="M287">
+        <v>4</v>
+      </c>
+      <c r="N287">
+        <v>4</v>
+      </c>
+      <c r="O287">
+        <v>18</v>
+      </c>
+      <c r="P287">
+        <v>19</v>
+      </c>
+      <c r="Q287">
+        <v>4</v>
+      </c>
+      <c r="R287">
+        <v>5</v>
+      </c>
+      <c r="S287">
+        <v>2</v>
+      </c>
+      <c r="T287">
+        <v>4</v>
+      </c>
+      <c r="U287">
+        <v>0</v>
+      </c>
+      <c r="V287">
+        <v>0</v>
+      </c>
+      <c r="W287">
+        <v>2.7</v>
+      </c>
+      <c r="X287">
+        <v>3.3</v>
+      </c>
+      <c r="Y287">
+        <v>2.6</v>
+      </c>
+      <c r="Z287">
+        <v>2.65</v>
+      </c>
+      <c r="AA287">
+        <v>3.1</v>
+      </c>
+      <c r="AB287">
+        <v>2.75</v>
+      </c>
+      <c r="AC287">
+        <v>2.65</v>
+      </c>
+      <c r="AD287">
+        <v>3.1</v>
+      </c>
+      <c r="AE287">
+        <v>2.75</v>
+      </c>
+      <c r="AF287">
+        <v>2.5</v>
+      </c>
+      <c r="AG287">
+        <v>3.3</v>
+      </c>
+      <c r="AH287">
+        <v>2.65</v>
+      </c>
+      <c r="AI287">
+        <v>2.6</v>
+      </c>
+      <c r="AJ287">
+        <v>3.3</v>
+      </c>
+      <c r="AK287">
+        <v>2.62</v>
+      </c>
+      <c r="AL287">
+        <v>2.88</v>
+      </c>
+      <c r="AM287">
+        <v>3.39</v>
+      </c>
+      <c r="AN287">
+        <v>2.65</v>
+      </c>
+      <c r="AO287">
+        <v>2.7</v>
+      </c>
+      <c r="AP287">
+        <v>3.1</v>
+      </c>
+      <c r="AQ287">
+        <v>2.7</v>
+      </c>
+      <c r="AR287">
+        <v>2.63</v>
+      </c>
+      <c r="AS287">
+        <v>3.25</v>
+      </c>
+      <c r="AT287">
+        <v>2.75</v>
+      </c>
+      <c r="AU287">
+        <v>2.8</v>
+      </c>
+      <c r="AV287">
+        <v>3.3</v>
+      </c>
+      <c r="AW287">
+        <v>2.62</v>
+      </c>
+      <c r="AX287">
+        <v>2.5</v>
+      </c>
+      <c r="AY287">
+        <v>3.3</v>
+      </c>
+      <c r="AZ287">
+        <v>2.75</v>
+      </c>
+      <c r="BA287">
+        <v>37</v>
+      </c>
+      <c r="BB287">
+        <v>2.88</v>
+      </c>
+      <c r="BC287">
+        <v>2.68</v>
+      </c>
+      <c r="BD287">
+        <v>3.4</v>
+      </c>
+      <c r="BE287">
+        <v>3.24</v>
+      </c>
+      <c r="BF287">
+        <v>2.75</v>
+      </c>
+      <c r="BG287">
+        <v>2.63</v>
+      </c>
+      <c r="BH287">
+        <v>36</v>
+      </c>
+      <c r="BI287">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BJ287">
+        <v>1.98</v>
+      </c>
+      <c r="BK287">
+        <v>1.9</v>
+      </c>
+      <c r="BL287">
+        <v>1.81</v>
+      </c>
+      <c r="BM287">
+        <v>19</v>
+      </c>
+      <c r="BN287">
+        <v>0</v>
+      </c>
+      <c r="BO287">
+        <v>2.04</v>
+      </c>
+      <c r="BP287">
+        <v>1.99</v>
+      </c>
+      <c r="BQ287">
+        <v>1.9</v>
+      </c>
+      <c r="BR287">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="288" spans="1:70">
+      <c r="A288" t="s">
+        <v>70</v>
+      </c>
+      <c r="B288" t="s">
+        <v>149</v>
+      </c>
+      <c r="C288" t="s">
+        <v>76</v>
+      </c>
+      <c r="D288" t="s">
+        <v>91</v>
+      </c>
+      <c r="E288">
+        <v>2</v>
+      </c>
+      <c r="F288">
+        <v>3</v>
+      </c>
+      <c r="G288" t="s">
+        <v>74</v>
+      </c>
+      <c r="H288">
+        <v>1</v>
+      </c>
+      <c r="I288">
+        <v>1</v>
+      </c>
+      <c r="J288" t="s">
+        <v>75</v>
+      </c>
+      <c r="K288">
+        <v>20</v>
+      </c>
+      <c r="L288">
+        <v>14</v>
+      </c>
+      <c r="M288">
+        <v>5</v>
+      </c>
+      <c r="N288">
+        <v>9</v>
+      </c>
+      <c r="O288">
+        <v>12</v>
+      </c>
+      <c r="P288">
+        <v>6</v>
+      </c>
+      <c r="Q288">
+        <v>10</v>
+      </c>
+      <c r="R288">
+        <v>4</v>
+      </c>
+      <c r="S288">
+        <v>3</v>
+      </c>
+      <c r="T288">
+        <v>2</v>
+      </c>
+      <c r="U288">
+        <v>0</v>
+      </c>
+      <c r="V288">
+        <v>0</v>
+      </c>
+      <c r="W288">
+        <v>1.91</v>
+      </c>
+      <c r="X288">
+        <v>3.5</v>
+      </c>
+      <c r="Y288">
+        <v>4</v>
+      </c>
+      <c r="Z288">
+        <v>1.87</v>
+      </c>
+      <c r="AA288">
+        <v>3.5</v>
+      </c>
+      <c r="AB288">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AC288">
+        <v>1.87</v>
+      </c>
+      <c r="AD288">
+        <v>3.5</v>
+      </c>
+      <c r="AE288">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AF288">
+        <v>2</v>
+      </c>
+      <c r="AG288">
+        <v>3.3</v>
+      </c>
+      <c r="AH288">
+        <v>3.6</v>
+      </c>
+      <c r="AI288">
+        <v>2</v>
+      </c>
+      <c r="AJ288">
+        <v>3.4</v>
+      </c>
+      <c r="AK288">
+        <v>3.75</v>
+      </c>
+      <c r="AL288">
+        <v>1.98</v>
+      </c>
+      <c r="AM288">
+        <v>3.6</v>
+      </c>
+      <c r="AN288">
+        <v>4.18</v>
+      </c>
+      <c r="AO288">
+        <v>2</v>
+      </c>
+      <c r="AP288">
+        <v>3.4</v>
+      </c>
+      <c r="AQ288">
+        <v>3.75</v>
+      </c>
+      <c r="AR288">
+        <v>2</v>
+      </c>
+      <c r="AS288">
+        <v>3.3</v>
+      </c>
+      <c r="AT288">
+        <v>4</v>
+      </c>
+      <c r="AU288">
+        <v>2</v>
+      </c>
+      <c r="AV288">
+        <v>3.6</v>
+      </c>
+      <c r="AW288">
+        <v>4</v>
+      </c>
+      <c r="AX288">
+        <v>2</v>
+      </c>
+      <c r="AY288">
+        <v>3.4</v>
+      </c>
+      <c r="AZ288">
+        <v>3.6</v>
+      </c>
+      <c r="BA288">
+        <v>38</v>
+      </c>
+      <c r="BB288">
+        <v>2</v>
+      </c>
+      <c r="BC288">
+        <v>1.95</v>
+      </c>
+      <c r="BD288">
+        <v>3.71</v>
+      </c>
+      <c r="BE288">
+        <v>3.41</v>
+      </c>
+      <c r="BF288">
+        <v>4.2</v>
+      </c>
+      <c r="BG288">
+        <v>3.9</v>
+      </c>
+      <c r="BH288">
+        <v>37</v>
+      </c>
+      <c r="BI288">
+        <v>2.1</v>
+      </c>
+      <c r="BJ288">
+        <v>1.98</v>
+      </c>
+      <c r="BK288">
+        <v>1.92</v>
+      </c>
+      <c r="BL288">
+        <v>1.82</v>
+      </c>
+      <c r="BM288">
+        <v>20</v>
+      </c>
+      <c r="BN288">
+        <v>-0.75</v>
+      </c>
+      <c r="BO288">
+        <v>2.34</v>
+      </c>
+      <c r="BP288">
+        <v>2.25</v>
+      </c>
+      <c r="BQ288">
+        <v>1.73</v>
+      </c>
+      <c r="BR288">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="289" spans="1:70">
+      <c r="A289" t="s">
+        <v>70</v>
+      </c>
+      <c r="B289" t="s">
+        <v>149</v>
+      </c>
+      <c r="C289" t="s">
+        <v>96</v>
+      </c>
+      <c r="D289" t="s">
+        <v>92</v>
+      </c>
+      <c r="E289">
+        <v>1</v>
+      </c>
+      <c r="F289">
+        <v>3</v>
+      </c>
+      <c r="G289" t="s">
+        <v>74</v>
+      </c>
+      <c r="H289">
+        <v>1</v>
+      </c>
+      <c r="I289">
+        <v>0</v>
+      </c>
+      <c r="J289" t="s">
+        <v>78</v>
+      </c>
+      <c r="K289">
+        <v>9</v>
+      </c>
+      <c r="L289">
+        <v>12</v>
+      </c>
+      <c r="M289">
+        <v>2</v>
+      </c>
+      <c r="N289">
+        <v>7</v>
+      </c>
+      <c r="O289">
+        <v>13</v>
+      </c>
+      <c r="P289">
+        <v>13</v>
+      </c>
+      <c r="Q289">
+        <v>11</v>
+      </c>
+      <c r="R289">
+        <v>7</v>
+      </c>
+      <c r="S289">
+        <v>1</v>
+      </c>
+      <c r="T289">
+        <v>1</v>
+      </c>
+      <c r="U289">
+        <v>0</v>
+      </c>
+      <c r="V289">
+        <v>0</v>
+      </c>
+      <c r="W289">
+        <v>2.1</v>
+      </c>
+      <c r="X289">
+        <v>3.2</v>
+      </c>
+      <c r="Y289">
+        <v>3.6</v>
+      </c>
+      <c r="Z289">
+        <v>2</v>
+      </c>
+      <c r="AA289">
+        <v>3.3</v>
+      </c>
+      <c r="AB289">
+        <v>3.8</v>
+      </c>
+      <c r="AC289">
+        <v>2</v>
+      </c>
+      <c r="AD289">
+        <v>3.3</v>
+      </c>
+      <c r="AE289">
+        <v>3.8</v>
+      </c>
+      <c r="AF289">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AG289">
+        <v>3.3</v>
+      </c>
+      <c r="AH289">
+        <v>3.5</v>
+      </c>
+      <c r="AI289">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AJ289">
+        <v>3.3</v>
+      </c>
+      <c r="AK289">
+        <v>3.6</v>
+      </c>
+      <c r="AL289">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AM289">
+        <v>3.31</v>
+      </c>
+      <c r="AN289">
+        <v>3.63</v>
+      </c>
+      <c r="AO289">
+        <v>2.25</v>
+      </c>
+      <c r="AP289">
+        <v>3.2</v>
+      </c>
+      <c r="AQ289">
+        <v>3.25</v>
+      </c>
+      <c r="AR289">
+        <v>2.1</v>
+      </c>
+      <c r="AS289">
+        <v>3.2</v>
+      </c>
+      <c r="AT289">
+        <v>3.75</v>
+      </c>
+      <c r="AU289">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AV289">
+        <v>3.3</v>
+      </c>
+      <c r="AW289">
+        <v>3.6</v>
+      </c>
+      <c r="AX289">
+        <v>2</v>
+      </c>
+      <c r="AY289">
+        <v>3.25</v>
+      </c>
+      <c r="AZ289">
+        <v>3.8</v>
+      </c>
+      <c r="BA289">
+        <v>38</v>
+      </c>
+      <c r="BB289">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BC289">
+        <v>2.14</v>
+      </c>
+      <c r="BD289">
+        <v>3.35</v>
+      </c>
+      <c r="BE289">
+        <v>3.24</v>
+      </c>
+      <c r="BF289">
+        <v>3.8</v>
+      </c>
+      <c r="BG289">
+        <v>3.53</v>
+      </c>
+      <c r="BH289">
+        <v>35</v>
+      </c>
+      <c r="BI289">
+        <v>2.34</v>
+      </c>
+      <c r="BJ289">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BK289">
+        <v>1.7</v>
+      </c>
+      <c r="BL289">
+        <v>1.65</v>
+      </c>
+      <c r="BM289">
+        <v>19</v>
+      </c>
+      <c r="BN289">
+        <v>-0.25</v>
+      </c>
+      <c r="BO289">
+        <v>1.92</v>
+      </c>
+      <c r="BP289">
+        <v>1.88</v>
+      </c>
+      <c r="BQ289">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BR289">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:70">
+      <c r="A290" t="s">
+        <v>70</v>
+      </c>
+      <c r="B290" s="1">
+        <v>41278</v>
+      </c>
+      <c r="C290" t="s">
+        <v>82</v>
+      </c>
+      <c r="D290" t="s">
+        <v>94</v>
+      </c>
+      <c r="E290">
+        <v>1</v>
+      </c>
+      <c r="F290">
+        <v>0</v>
+      </c>
+      <c r="G290" t="s">
+        <v>78</v>
+      </c>
+      <c r="H290">
+        <v>0</v>
+      </c>
+      <c r="I290">
+        <v>0</v>
+      </c>
+      <c r="J290" t="s">
+        <v>75</v>
+      </c>
+      <c r="K290">
+        <v>14</v>
+      </c>
+      <c r="L290">
+        <v>7</v>
+      </c>
+      <c r="M290">
+        <v>4</v>
+      </c>
+      <c r="N290">
+        <v>3</v>
+      </c>
+      <c r="O290">
+        <v>14</v>
+      </c>
+      <c r="P290">
+        <v>19</v>
+      </c>
+      <c r="Q290">
+        <v>3</v>
+      </c>
+      <c r="R290">
+        <v>8</v>
+      </c>
+      <c r="S290">
+        <v>1</v>
+      </c>
+      <c r="T290">
+        <v>1</v>
+      </c>
+      <c r="U290">
+        <v>1</v>
+      </c>
+      <c r="V290">
+        <v>0</v>
+      </c>
+      <c r="W290">
+        <v>1.73</v>
+      </c>
+      <c r="X290">
+        <v>3.6</v>
+      </c>
+      <c r="Y290">
+        <v>4.75</v>
+      </c>
+      <c r="Z290">
+        <v>1.75</v>
+      </c>
+      <c r="AA290">
+        <v>3.7</v>
+      </c>
+      <c r="AB290">
+        <v>4.5</v>
+      </c>
+      <c r="AC290">
+        <v>1.75</v>
+      </c>
+      <c r="AD290">
+        <v>3.7</v>
+      </c>
+      <c r="AE290">
+        <v>4.5</v>
+      </c>
+      <c r="AF290">
+        <v>1.75</v>
+      </c>
+      <c r="AG290">
+        <v>3.5</v>
+      </c>
+      <c r="AH290">
+        <v>4.5</v>
+      </c>
+      <c r="AI290">
+        <v>1.75</v>
+      </c>
+      <c r="AJ290">
+        <v>3.75</v>
+      </c>
+      <c r="AK290">
+        <v>4.5</v>
+      </c>
+      <c r="AL290">
+        <v>1.75</v>
+      </c>
+      <c r="AM290">
+        <v>3.98</v>
+      </c>
+      <c r="AN290">
+        <v>5.08</v>
+      </c>
+      <c r="AO290">
+        <v>1.75</v>
+      </c>
+      <c r="AP290">
+        <v>3.6</v>
+      </c>
+      <c r="AQ290">
+        <v>4.75</v>
+      </c>
+      <c r="AR290">
+        <v>1.73</v>
+      </c>
+      <c r="AS290">
+        <v>3.75</v>
+      </c>
+      <c r="AT290">
+        <v>4.8</v>
+      </c>
+      <c r="AU290">
+        <v>1.75</v>
+      </c>
+      <c r="AV290">
+        <v>3.9</v>
+      </c>
+      <c r="AW290">
+        <v>4.8</v>
+      </c>
+      <c r="AX290">
+        <v>1.75</v>
+      </c>
+      <c r="AY290">
+        <v>3.6</v>
+      </c>
+      <c r="AZ290">
+        <v>4.5</v>
+      </c>
+      <c r="BA290">
+        <v>37</v>
+      </c>
+      <c r="BB290">
+        <v>1.78</v>
+      </c>
+      <c r="BC290">
+        <v>1.73</v>
+      </c>
+      <c r="BD290">
+        <v>3.98</v>
+      </c>
+      <c r="BE290">
+        <v>3.71</v>
+      </c>
+      <c r="BF290">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="BG290">
+        <v>4.72</v>
+      </c>
+      <c r="BH290">
+        <v>36</v>
+      </c>
+      <c r="BI290">
+        <v>1.88</v>
+      </c>
+      <c r="BJ290">
+        <v>1.81</v>
+      </c>
+      <c r="BK290">
+        <v>2.1</v>
+      </c>
+      <c r="BL290">
+        <v>1.98</v>
+      </c>
+      <c r="BM290">
+        <v>21</v>
+      </c>
+      <c r="BN290">
+        <v>-0.75</v>
+      </c>
+      <c r="BO290">
+        <v>1.98</v>
+      </c>
+      <c r="BP290">
+        <v>1.94</v>
+      </c>
+      <c r="BQ290">
+        <v>1.98</v>
+      </c>
+      <c r="BR290">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="291" spans="1:70">
+      <c r="A291" t="s">
+        <v>70</v>
+      </c>
+      <c r="B291" s="1">
+        <v>41278</v>
+      </c>
+      <c r="C291" t="s">
+        <v>83</v>
+      </c>
+      <c r="D291" t="s">
+        <v>80</v>
+      </c>
+      <c r="E291">
+        <v>0</v>
+      </c>
+      <c r="F291">
+        <v>0</v>
+      </c>
+      <c r="G291" t="s">
+        <v>75</v>
+      </c>
+      <c r="H291">
+        <v>0</v>
+      </c>
+      <c r="I291">
+        <v>0</v>
+      </c>
+      <c r="J291" t="s">
+        <v>75</v>
+      </c>
+      <c r="K291">
+        <v>8</v>
+      </c>
+      <c r="L291">
+        <v>16</v>
+      </c>
+      <c r="M291">
+        <v>4</v>
+      </c>
+      <c r="N291">
+        <v>7</v>
+      </c>
+      <c r="O291">
+        <v>13</v>
+      </c>
+      <c r="P291">
+        <v>10</v>
+      </c>
+      <c r="Q291">
+        <v>6</v>
+      </c>
+      <c r="R291">
+        <v>5</v>
+      </c>
+      <c r="S291">
+        <v>4</v>
+      </c>
+      <c r="T291">
+        <v>2</v>
+      </c>
+      <c r="U291">
+        <v>0</v>
+      </c>
+      <c r="V291">
+        <v>0</v>
+      </c>
+      <c r="W291">
+        <v>1.83</v>
+      </c>
+      <c r="X291">
+        <v>3.6</v>
+      </c>
+      <c r="Y291">
+        <v>4.2</v>
+      </c>
+      <c r="Z291">
+        <v>1.88</v>
+      </c>
+      <c r="AA291">
+        <v>3.4</v>
+      </c>
+      <c r="AB291">
+        <v>4.2</v>
+      </c>
+      <c r="AC291">
+        <v>1.88</v>
+      </c>
+      <c r="AD291">
+        <v>3.4</v>
+      </c>
+      <c r="AE291">
+        <v>4.2</v>
+      </c>
+      <c r="AF291">
+        <v>2</v>
+      </c>
+      <c r="AG291">
+        <v>3.3</v>
+      </c>
+      <c r="AH291">
+        <v>3.6</v>
+      </c>
+      <c r="AI291">
+        <v>1.9</v>
+      </c>
+      <c r="AJ291">
+        <v>3.5</v>
+      </c>
+      <c r="AK291">
+        <v>3.8</v>
+      </c>
+      <c r="AL291">
+        <v>1.89</v>
+      </c>
+      <c r="AM291">
+        <v>3.64</v>
+      </c>
+      <c r="AN291">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="AO291">
+        <v>1.85</v>
+      </c>
+      <c r="AP291">
+        <v>3.4</v>
+      </c>
+      <c r="AQ291">
+        <v>4.33</v>
+      </c>
+      <c r="AR291">
+        <v>1.91</v>
+      </c>
+      <c r="AS291">
+        <v>3.5</v>
+      </c>
+      <c r="AT291">
+        <v>4</v>
+      </c>
+      <c r="AU291">
+        <v>1.91</v>
+      </c>
+      <c r="AV291">
+        <v>3.6</v>
+      </c>
+      <c r="AW291">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AX291">
+        <v>1.95</v>
+      </c>
+      <c r="AY291">
+        <v>3.5</v>
+      </c>
+      <c r="AZ291">
+        <v>3.75</v>
+      </c>
+      <c r="BA291">
+        <v>37</v>
+      </c>
+      <c r="BB291">
+        <v>2</v>
+      </c>
+      <c r="BC291">
+        <v>1.88</v>
+      </c>
+      <c r="BD291">
+        <v>3.64</v>
+      </c>
+      <c r="BE291">
+        <v>3.44</v>
+      </c>
+      <c r="BF291">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="BG291">
+        <v>4.18</v>
+      </c>
+      <c r="BH291">
+        <v>36</v>
+      </c>
+      <c r="BI291">
+        <v>2.11</v>
+      </c>
+      <c r="BJ291">
+        <v>2.02</v>
+      </c>
+      <c r="BK291">
+        <v>1.89</v>
+      </c>
+      <c r="BL291">
+        <v>1.79</v>
+      </c>
+      <c r="BM291">
+        <v>20</v>
+      </c>
+      <c r="BN291">
+        <v>-0.75</v>
+      </c>
+      <c r="BO291">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="BP291">
+        <v>2.12</v>
+      </c>
+      <c r="BQ291">
+        <v>1.82</v>
+      </c>
+      <c r="BR291">
+        <v>1.77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>